<commit_message>
📊 Update Orders.xlsx from orders.jsonl
</commit_message>
<xml_diff>
--- a/data/Orders.xlsx
+++ b/data/Orders.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,6 +517,90 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ORD-2025002</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>فاطمة محمود</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0559876543</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>أبو ظبي</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>عطر فرنسي + شمعات عطرة</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>350 AED</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2025-12-13</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2025-12-13T17:10:00Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ORD-2025003</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>علي محمد</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0507654321</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>الشارقة</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>ساعة ذهبية + بطاقة u03hf</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>500 AED</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2025-12-13</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2025-12-13T17:20:00Z</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>